<commit_message>
ze pequeno eletro matriz
</commit_message>
<xml_diff>
--- a/as-is-documentation/ze-pequeno-eletro.xlsx
+++ b/as-is-documentation/ze-pequeno-eletro.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="What - Perspectiva Executiva" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t xml:space="preserve">Glossário de termos de negócio</t>
   </si>
@@ -144,22 +144,28 @@
     <t xml:space="preserve">Centro de Distribuição </t>
   </si>
   <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Legenda:</t>
   </si>
   <si>
-    <t xml:space="preserve">C = consome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P = produz</t>
+    <t xml:space="preserve">C = Cria / Create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R = Lê / Read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U = Atualiza / Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D = Remove / Delete</t>
   </si>
   <si>
     <t xml:space="preserve">Aplicações</t>
@@ -393,7 +399,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -492,6 +498,10 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -752,11 +762,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="103.09"/>
@@ -871,7 +881,7 @@
       <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.57"/>
@@ -999,15 +1009,15 @@
   </sheetPr>
   <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H26" activeCellId="0" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.7"/>
@@ -1015,7 +1025,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="103.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.66"/>
@@ -1061,12 +1071,12 @@
         <v>40</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="I2" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1084,22 +1094,26 @@
       </c>
       <c r="G3" s="16"/>
       <c r="I3" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
+      <c r="B4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="D4" s="12" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="14"/>
       <c r="G4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>45</v>
@@ -1109,26 +1123,38 @@
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
+      <c r="I5" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="C6" s="19"/>
-      <c r="D6" s="16"/>
+      <c r="D6" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="19"/>
       <c r="G6" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1161,7 +1187,7 @@
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>2</v>
@@ -1174,7 +1200,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
@@ -1191,10 +1217,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -1207,10 +1233,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -1223,10 +1249,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
@@ -1239,10 +1265,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
@@ -1253,15 +1279,35 @@
       <c r="I14" s="24"/>
       <c r="J14" s="12"/>
     </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+    </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
     </row>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>